<commit_message>
corrections in the vocabulary
</commit_message>
<xml_diff>
--- a/data-raw/Vocabulary.xlsx
+++ b/data-raw/Vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{249DC122-4B69-417D-93DE-81021C0D660E}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{21E25AD4-E50C-4DF6-A117-C5FCFCC90211}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="6" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="factor_binary" sheetId="1" r:id="rId1"/>
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9CFAA-61F8-4C56-BD85-7E9D727436E0}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,10 +1497,10 @@
         <v>250</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,10 +1508,10 @@
         <v>251</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,11 +1661,11 @@
       <c r="A20" t="s">
         <v>265</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C20" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2888,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D578B6A3-7F47-4CB1-924B-8B05ABD288B1}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
not yet well documented new reader function
</commit_message>
<xml_diff>
--- a/data-raw/Vocabulary.xlsx
+++ b/data-raw/Vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="532" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{171C92B8-6E9D-4A96-B7CF-BBB32BD453FD}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{6A50BBBE-F810-4CD6-9EC4-8C9119E7E325}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="factor_binary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="416">
   <si>
     <t>Inefficient</t>
   </si>
@@ -1261,6 +1261,24 @@
   </si>
   <si>
     <t>large town</t>
+  </si>
+  <si>
+    <t>false (correct)</t>
+  </si>
+  <si>
+    <t>true.</t>
+  </si>
+  <si>
+    <t>true2</t>
+  </si>
+  <si>
+    <t>false.</t>
+  </si>
+  <si>
+    <t>true (correct)</t>
+  </si>
+  <si>
+    <t>true3</t>
   </si>
 </sst>
 </file>
@@ -1631,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9CFAA-61F8-4C56-BD85-7E9D727436E0}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,6 +1902,28 @@
       </c>
       <c r="C22" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>412</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C23" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>415</v>
+      </c>
+      <c r="B24" t="s">
+        <v>413</v>
+      </c>
+      <c r="C24" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2354,7 +2394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A2899-80DE-49F6-A1F5-04E9760B495F}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Creating a single vocabulary file
</commit_message>
<xml_diff>
--- a/data-raw/Vocabulary.xlsx
+++ b/data-raw/Vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="555" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{AA5F1D74-5C81-4CDE-8B2F-E918C6390D2C}"/>
+  <xr:revisionPtr revIDLastSave="601" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{456312E5-6871-42EC-AE25-C40D9B4A97D7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="factor_binary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="407">
   <si>
     <t>Inefficient</t>
   </si>
@@ -114,15 +114,6 @@
     <t>disagree</t>
   </si>
   <si>
-    <t>factor_3_0</t>
-  </si>
-  <si>
-    <t>factor_3_1</t>
-  </si>
-  <si>
-    <t>factor_3_2</t>
-  </si>
-  <si>
     <t>No, probably not</t>
   </si>
   <si>
@@ -279,27 +270,6 @@
     <t>Very negative view</t>
   </si>
   <si>
-    <t>yes_2_value</t>
-  </si>
-  <si>
-    <t>yes_1_value</t>
-  </si>
-  <si>
-    <t>no_1_value</t>
-  </si>
-  <si>
-    <t>no_2_value</t>
-  </si>
-  <si>
-    <t>factor_positive</t>
-  </si>
-  <si>
-    <t>factor_null</t>
-  </si>
-  <si>
-    <t>factor_negative</t>
-  </si>
-  <si>
     <t>Too little</t>
   </si>
   <si>
@@ -441,18 +411,6 @@
     <t>Neither the one nor the other (SPONTANEOUS)</t>
   </si>
   <si>
-    <t>factor_4_0</t>
-  </si>
-  <si>
-    <t>factor_4_1</t>
-  </si>
-  <si>
-    <t>factor_4_2</t>
-  </si>
-  <si>
-    <t>factor_4_3</t>
-  </si>
-  <si>
     <t>Not at all</t>
   </si>
   <si>
@@ -813,12 +771,6 @@
     <t>efficient1</t>
   </si>
   <si>
-    <t>positive_values</t>
-  </si>
-  <si>
-    <t>negative_values</t>
-  </si>
-  <si>
     <t>good_bad_4_1</t>
   </si>
   <si>
@@ -855,9 +807,6 @@
     <t>certainly_4_1</t>
   </si>
   <si>
-    <t>little_much_3</t>
-  </si>
-  <si>
     <t>amount_3_1</t>
   </si>
   <si>
@@ -939,9 +888,6 @@
     <t>tension_3_1</t>
   </si>
   <si>
-    <t>Strong_3_1</t>
-  </si>
-  <si>
     <t>society_3_1</t>
   </si>
   <si>
@@ -1005,21 +951,6 @@
     <t>good_4_1</t>
   </si>
   <si>
-    <t>factor_5_0</t>
-  </si>
-  <si>
-    <t>factor_5_1</t>
-  </si>
-  <si>
-    <t>factor_5_2</t>
-  </si>
-  <si>
-    <t>factor_5_3</t>
-  </si>
-  <si>
-    <t>factor_5_4</t>
-  </si>
-  <si>
     <t>More or less the same</t>
   </si>
   <si>
@@ -1044,9 +975,6 @@
     <t>n_of_persons_present_during_interview</t>
   </si>
   <si>
-    <t xml:space="preserve"> level_in_society_self_placement</t>
-  </si>
-  <si>
     <t>Much better</t>
   </si>
   <si>
@@ -1194,9 +1122,6 @@
     <t>Not important</t>
   </si>
   <si>
-    <t>important_2</t>
-  </si>
-  <si>
     <t>agree2</t>
   </si>
   <si>
@@ -1224,9 +1149,6 @@
     <t>strong_4_2</t>
   </si>
   <si>
-    <t>agree5_1</t>
-  </si>
-  <si>
     <t>Adequate</t>
   </si>
   <si>
@@ -1288,6 +1210,48 @@
   </si>
   <si>
     <t>informed_3_1</t>
+  </si>
+  <si>
+    <t>level_in_society_self_placement</t>
+  </si>
+  <si>
+    <t>pos_1</t>
+  </si>
+  <si>
+    <t>neg_1</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>pos_2</t>
+  </si>
+  <si>
+    <t>neg_2</t>
+  </si>
+  <si>
+    <t>pos_3</t>
+  </si>
+  <si>
+    <t>good_bad_3_4</t>
+  </si>
+  <si>
+    <t>positive_4_2</t>
+  </si>
+  <si>
+    <t>risk_4_1</t>
+  </si>
+  <si>
+    <t>agree_5_1</t>
+  </si>
+  <si>
+    <t>important1</t>
+  </si>
+  <si>
+    <t>little_much_3_1</t>
+  </si>
+  <si>
+    <t>well_4_1</t>
   </si>
 </sst>
 </file>
@@ -1660,8 +1624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9CFAA-61F8-4C56-BD85-7E9D727436E0}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,269 +1638,272 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>394</v>
       </c>
       <c r="C1" t="s">
-        <v>261</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>363</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>347</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>345</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>254</v>
+        <v>404</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
+        <v>361</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
+        <v>170</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="B18" t="s">
-        <v>186</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>258</v>
-      </c>
-      <c r="B19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>185</v>
+        <v>232</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>371</v>
-      </c>
-      <c r="B20" t="s">
-        <v>369</v>
+        <v>386</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>384</v>
       </c>
       <c r="C20" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>389</v>
+      </c>
+      <c r="B21" t="s">
         <v>387</v>
       </c>
-      <c r="B21" t="s">
-        <v>385</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>386</v>
+      <c r="C21" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>388</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>412</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>410</v>
+        <v>230</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>411</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>415</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>413</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>414</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C24">
+    <sortCondition ref="A2:A24"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1945,13 +1913,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03697B1-1619-4CB8-8AA4-B6550CA28181}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
@@ -1959,114 +1928,114 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>394</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>396</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>352</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>353</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>350</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>327</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,111 +2043,111 @@
         <v>276</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>346</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>344</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
-        <v>345</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>296</v>
+        <v>400</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>322</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>320</v>
       </c>
       <c r="D13" t="s">
-        <v>220</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>291</v>
+        <v>355</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,214 +2155,214 @@
         <v>274</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>284</v>
+        <v>356</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>283</v>
+        <v>405</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
         <v>120</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>121</v>
-      </c>
-      <c r="D22" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
         <v>205</v>
       </c>
       <c r="C23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>294</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>298</v>
+        <v>273</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>299</v>
+        <v>189</v>
+      </c>
+      <c r="D26" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B27" t="s">
-        <v>222</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>349</v>
+        <v>269</v>
       </c>
       <c r="B28" t="s">
-        <v>348</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>372</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>379</v>
-      </c>
-      <c r="B30" t="s">
-        <v>132</v>
+        <v>277</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" t="s">
-        <v>134</v>
+        <v>209</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>400</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
-        <v>398</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
-        <v>399</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D27">
-    <sortCondition ref="A2:A27"/>
+  <sortState ref="A2:D31">
+    <sortCondition ref="A2:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2403,8 +2372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A2899-80DE-49F6-A1F5-04E9760B495F}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,187 +2387,190 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>396</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>394</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
+        <v>342</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>307</v>
+        <v>392</v>
       </c>
       <c r="B6" t="s">
-        <v>366</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>364</v>
+        <v>391</v>
+      </c>
+      <c r="C6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>406</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>229</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>304</v>
+        <v>275</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>305</v>
+        <v>380</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>407</v>
+        <v>381</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
       <c r="D12" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>418</v>
+        <v>284</v>
       </c>
       <c r="B13" t="s">
-        <v>417</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>416</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D13">
+    <sortCondition ref="A2:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2608,7 +2581,8 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2622,345 +2596,348 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>397</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>394</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>395</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>330</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>334</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>181</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>379</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>376</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>378</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>377</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>337</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>335</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" t="s">
         <v>358</v>
       </c>
-      <c r="D12" t="s">
-        <v>357</v>
-      </c>
       <c r="E12" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>363</v>
+        <v>401</v>
       </c>
       <c r="B16" t="s">
-        <v>362</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>361</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>359</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>360</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>256</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>384</v>
+        <v>254</v>
       </c>
       <c r="B18" t="s">
-        <v>381</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>383</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>382</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>366</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>393</v>
+        <v>247</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>405</v>
+        <v>255</v>
       </c>
       <c r="B20" t="s">
-        <v>402</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>404</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>403</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>401</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E20">
+    <sortCondition ref="A2:A20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2969,8 +2946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46AE99A-EA61-4837-A6C5-82AEF03E78CB}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="A24:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2984,399 +2962,402 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>396</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>394</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>397</v>
       </c>
       <c r="E1" t="s">
-        <v>139</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>313</v>
+        <v>364</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
-        <v>158</v>
+        <v>361</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>322</v>
+        <v>256</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>342</v>
       </c>
       <c r="C13" t="s">
-        <v>181</v>
+        <v>354</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>341</v>
       </c>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>367</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>365</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>317</v>
-      </c>
-      <c r="B15" t="s">
-        <v>194</v>
+        <v>402</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="E15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>321</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>199</v>
+        <v>303</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>211</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>376</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
-        <v>375</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
-        <v>372</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>373</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>374</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>272</v>
+        <v>371</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D20" t="s">
-        <v>365</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>389</v>
+        <v>352</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>348</v>
       </c>
       <c r="D21" t="s">
-        <v>385</v>
+        <v>349</v>
       </c>
       <c r="E21" t="s">
-        <v>151</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="C22" t="s">
-        <v>390</v>
+        <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="E22" t="s">
-        <v>391</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>396</v>
+        <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>394</v>
+        <v>163</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="E23" t="s">
-        <v>395</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3387,11 +3368,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
@@ -3401,105 +3384,108 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>324</v>
+        <v>398</v>
       </c>
       <c r="C1" t="s">
-        <v>325</v>
+        <v>395</v>
       </c>
       <c r="D1" t="s">
-        <v>326</v>
+        <v>396</v>
       </c>
       <c r="E1" t="s">
-        <v>327</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>328</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>403</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>332</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>329</v>
+        <v>189</v>
       </c>
       <c r="E2" t="s">
-        <v>333</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>330</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C3" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="D3" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="F3" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>311</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>308</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>367</v>
+        <v>306</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>310</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>397</v>
+        <v>344</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>343</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F5">
+    <sortCondition ref="A2:A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3509,29 +3495,29 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new raw vocabulary file
</commit_message>
<xml_diff>
--- a/data-raw/Vocabulary.xlsx
+++ b/data-raw/Vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="601" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{456312E5-6871-42EC-AE25-C40D9B4A97D7}"/>
+  <xr:revisionPtr revIDLastSave="602" documentId="8_{1F982E31-BC7A-450F-8AC7-346FCF11D38C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{ED14556C-170C-43E5-9CEB-A11CF9094B47}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{F0E7EEBB-22F3-4EFF-9ECF-DA45CE23BB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="factor_binary" sheetId="1" r:id="rId1"/>
@@ -2370,11 +2370,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A2899-80DE-49F6-A1F5-04E9760B495F}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2554,22 +2554,25 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>284</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>200</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>198</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D13">
-    <sortCondition ref="A2:A13"/>
+  <sortState ref="A2:D14">
+    <sortCondition ref="A2:A14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2946,7 +2949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46AE99A-EA61-4837-A6C5-82AEF03E78CB}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>

</xml_diff>